<commit_message>
Modify wireshark from blackList to whiteList
</commit_message>
<xml_diff>
--- a/vulsList_20160128.xlsx
+++ b/vulsList_20160128.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<s:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <s:workbookPr codeName="ThisWorkbook"/>
-  <s:bookViews>
-    <s:workbookView activeTab="3"/>
-  </s:bookViews>
-  <s:sheets>
-    <s:sheet name="whiteList" sheetId="1" r:id="rId1"/>
-    <s:sheet name="blackList" sheetId="2" r:id="rId2"/>
-    <s:sheet name="vulsHistory" sheetId="3" r:id="rId3"/>
-    <s:sheet name="vuls" sheetId="4" r:id="rId4"/>
-  </s:sheets>
-  <s:definedNames/>
-  <s:calcPr calcId="124519" fullCalcOnLoad="1"/>
-</s:workbook>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <bookViews>
+    <workbookView xWindow="570" yWindow="465" windowWidth="8280" windowHeight="6960" activeTab="1"/>
+  </bookViews>
+  <sheets>
+    <sheet name="whiteList" sheetId="1" r:id="rId1"/>
+    <sheet name="blackList" sheetId="2" r:id="rId2"/>
+    <sheet name="vulsHistory" sheetId="3" r:id="rId3"/>
+    <sheet name="vuls" sheetId="4" r:id="rId4"/>
+  </sheets>
+  <calcPr calcId="125725"/>
+</workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="500">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="943" uniqueCount="500">
   <si>
     <t>tech keywords</t>
   </si>
@@ -1524,51 +1524,38 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt formatCode="yyyy-mm-dd h:mm:ss" numFmtId="164"/>
+    <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
   </numFmts>
   <fonts count="3">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="新細明體"/>
+      <family val="2"/>
       <charset val="136"/>
-      <family val="2"/>
-      <color theme="1"/>
-      <sz val="12"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="微軟正黑體"/>
+      <family val="2"/>
+      <charset val="136"/>
+    </font>
+    <font>
+      <sz val="9"/>
       <name val="新細明體"/>
+      <family val="2"/>
       <charset val="136"/>
-      <family val="2"/>
-      <color rgb="00000000"/>
-      <sz val="9"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <name val="微軟正黑體"/>
-      <charset val="136"/>
-      <family val="2"/>
-      <color theme="1"/>
-      <sz val="12"/>
-    </font>
   </fonts>
-  <fills count="7">
+  <fills count="5">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="43"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="47"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -1599,47 +1586,31 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+  <cellXfs count="10">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="14" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="3" fontId="0" numFmtId="14" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="3" fontId="0" numFmtId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="4" fontId="0" numFmtId="164" xfId="0"/>
-    <xf borderId="0" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="5" fontId="0" numFmtId="164" xfId="0"/>
-    <xf borderId="0" fillId="5" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
-    <xf borderId="0" fillId="6" fontId="0" numFmtId="164" xfId="0"/>
-    <xf borderId="0" fillId="6" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="176" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="176" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="一般" xfId="0"/>
+    <cellStyle name="一般" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
@@ -1927,22 +1898,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="1" width="17.375"/>
-    <col customWidth="1" max="2" min="2" style="1" width="9.375"/>
-    <col customWidth="1" max="16384" min="3" style="1" width="9"/>
+    <col min="1" max="1" width="17.375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -2065,28 +2033,31 @@
         <v>23</v>
       </c>
     </row>
+    <row r="25" spans="1:1">
+      <c r="A25" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="200" orientation="portrait" paperSize="9" verticalDpi="200"/>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="1" width="15.375"/>
-    <col customWidth="1" max="16384" min="2" style="1" width="9"/>
+    <col min="1" max="1" width="15.375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -2134,30 +2105,20 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
-      <c r="A10" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="200" orientation="portrait" paperSize="9" verticalDpi="200"/>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G84"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="16.5"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
@@ -2183,209 +2144,209 @@
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="9" t="n">
+      <c r="A2" s="3">
         <v>42387</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="E2" s="10" t="n"/>
-      <c r="F2" s="10" t="n"/>
-      <c r="G2" s="10" t="s">
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="9" t="n">
+      <c r="A3" s="3">
         <v>42387</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="E3" s="10" t="n"/>
-      <c r="F3" s="10" t="n"/>
-      <c r="G3" s="10" t="s">
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="9" t="n">
+      <c r="A4" s="3">
         <v>42387</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E4" s="10" t="n"/>
-      <c r="F4" s="10" t="n"/>
-      <c r="G4" s="10" t="s">
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="9" t="n">
+      <c r="A5" s="3">
         <v>42387</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="F5" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="G5" s="10" t="s">
+      <c r="F5" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G5" s="4" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="14" t="n">
+      <c r="A6" s="8">
         <v>42384</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="15" t="s">
+      <c r="D6" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="E6" s="15" t="n"/>
-      <c r="F6" s="15" t="n"/>
-      <c r="G6" s="15" t="s">
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="9" t="n">
+      <c r="A7" s="3">
         <v>42384</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="E7" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="F7" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="G7" s="10" t="s">
+      <c r="F7" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G7" s="4" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="9" t="n">
+      <c r="A8" s="3">
         <v>42384</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="E8" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="F8" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="G8" s="10" t="s">
+      <c r="F8" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G8" s="4" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="9" t="n">
+      <c r="A9" s="3">
         <v>42383</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="E9" s="10" t="n"/>
-      <c r="F9" s="10" t="n"/>
-      <c r="G9" s="10" t="s">
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="9" t="n">
+      <c r="A10" s="3">
         <v>42383</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="D10" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="E10" s="10" t="n"/>
-      <c r="F10" s="10" t="n"/>
-      <c r="G10" s="10" t="s">
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="9" t="n">
+      <c r="A11" s="3">
         <v>42383</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="D11" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="E11" s="10" t="n"/>
-      <c r="F11" s="10" t="n"/>
-      <c r="G11" s="10" t="s">
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="13" t="n">
+      <c r="A12" s="7">
         <v>42388</v>
       </c>
       <c r="B12" t="s">
@@ -2408,142 +2369,142 @@
       </c>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="9" t="n">
+      <c r="A13" s="3">
         <v>42387</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="D13" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="E13" s="10" t="n"/>
-      <c r="F13" s="10" t="n"/>
-      <c r="G13" s="10" t="s">
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="9" t="n">
+      <c r="A14" s="3">
         <v>42384</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="C14" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="D14" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="E14" s="10" t="n"/>
-      <c r="F14" s="10" t="n"/>
-      <c r="G14" s="10" t="s">
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="9" t="n">
+      <c r="A15" s="3">
         <v>42388</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="C15" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D15" s="10" t="s">
+      <c r="D15" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="E15" s="10" t="n"/>
-      <c r="F15" s="10" t="n"/>
-      <c r="G15" s="10" t="s">
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="9" t="n">
+      <c r="A16" s="3">
         <v>42384</v>
       </c>
-      <c r="B16" s="10" t="s">
+      <c r="B16" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C16" s="10" t="s">
+      <c r="C16" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D16" s="10" t="s">
+      <c r="D16" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="E16" s="10" t="n"/>
-      <c r="F16" s="10" t="n"/>
-      <c r="G16" s="10" t="s">
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="9" t="n">
+      <c r="A17" s="3">
         <v>42389</v>
       </c>
-      <c r="B17" s="10" t="s">
+      <c r="B17" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="C17" s="10" t="n"/>
-      <c r="D17" s="10" t="s">
+      <c r="C17" s="4"/>
+      <c r="D17" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="E17" s="10" t="s">
+      <c r="E17" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="F17" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="G17" s="10" t="s">
+      <c r="F17" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G17" s="4" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="9" t="n">
+      <c r="A18" s="3">
         <v>42389</v>
       </c>
-      <c r="B18" s="10" t="s">
+      <c r="B18" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="C18" s="10" t="n"/>
-      <c r="D18" s="10" t="s">
+      <c r="C18" s="4"/>
+      <c r="D18" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="E18" s="10" t="n"/>
-      <c r="F18" s="10" t="n"/>
-      <c r="G18" s="10" t="s">
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="9" t="n">
+      <c r="A19" s="3">
         <v>42384</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="B19" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="C19" s="10" t="n"/>
-      <c r="D19" s="10" t="s">
+      <c r="C19" s="4"/>
+      <c r="D19" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="E19" s="10" t="s">
+      <c r="E19" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="F19" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="G19" s="10" t="s">
+      <c r="F19" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G19" s="4" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" s="13" t="n">
+      <c r="A20" s="7">
         <v>42384</v>
       </c>
       <c r="B20" t="s">
@@ -2566,24 +2527,24 @@
       </c>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="9" t="n">
+      <c r="A21" s="3">
         <v>42383</v>
       </c>
-      <c r="B21" s="10" t="s">
+      <c r="B21" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="C21" s="10" t="n"/>
-      <c r="D21" s="10" t="s">
+      <c r="C21" s="4"/>
+      <c r="D21" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="E21" s="10" t="n"/>
-      <c r="F21" s="10" t="n"/>
-      <c r="G21" s="10" t="s">
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:7">
-      <c r="A22" s="13" t="n">
+      <c r="A22" s="7">
         <v>42389</v>
       </c>
       <c r="B22" t="s">
@@ -2606,110 +2567,110 @@
       </c>
     </row>
     <row r="23" spans="1:7">
-      <c r="A23" s="9" t="n">
+      <c r="A23" s="3">
         <v>42389</v>
       </c>
-      <c r="B23" s="10" t="s">
+      <c r="B23" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="C23" s="10" t="n"/>
-      <c r="D23" s="10" t="s">
+      <c r="C23" s="4"/>
+      <c r="D23" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="E23" s="10" t="s">
+      <c r="E23" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="F23" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="G23" s="10" t="s">
+      <c r="F23" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G23" s="4" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="24" spans="1:7">
-      <c r="A24" s="11" t="n">
+      <c r="A24" s="5">
         <v>42389</v>
       </c>
-      <c r="B24" s="12" t="s">
+      <c r="B24" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="C24" s="12" t="n"/>
-      <c r="D24" s="12" t="s">
+      <c r="C24" s="6"/>
+      <c r="D24" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="E24" s="12" t="s">
+      <c r="E24" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="F24" s="12" t="n"/>
-      <c r="G24" s="12" t="s">
+      <c r="F24" s="6"/>
+      <c r="G24" s="6" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="25" spans="1:7">
-      <c r="A25" s="9" t="n">
+      <c r="A25" s="3">
         <v>42389</v>
       </c>
-      <c r="B25" s="10" t="s">
+      <c r="B25" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C25" s="10" t="n"/>
-      <c r="D25" s="10" t="s">
+      <c r="C25" s="4"/>
+      <c r="D25" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="E25" s="10" t="s">
+      <c r="E25" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="F25" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="G25" s="10" t="s">
+      <c r="F25" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G25" s="4" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="26" spans="1:7">
-      <c r="A26" s="9" t="n">
+      <c r="A26" s="3">
         <v>42388</v>
       </c>
-      <c r="B26" s="10" t="s">
+      <c r="B26" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="C26" s="10" t="n"/>
-      <c r="D26" s="10" t="s">
+      <c r="C26" s="4"/>
+      <c r="D26" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="E26" s="10" t="s">
+      <c r="E26" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="F26" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="G26" s="10" t="s">
+      <c r="F26" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G26" s="4" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:7">
-      <c r="A27" s="9" t="n">
+      <c r="A27" s="3">
         <v>42388</v>
       </c>
-      <c r="B27" s="10" t="s">
+      <c r="B27" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="C27" s="10" t="n"/>
-      <c r="D27" s="10" t="s">
+      <c r="C27" s="4"/>
+      <c r="D27" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="E27" s="10" t="s">
+      <c r="E27" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="F27" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="G27" s="10" t="s">
+      <c r="F27" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G27" s="4" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="28" spans="1:7">
-      <c r="A28" s="13" t="n">
+      <c r="A28" s="7">
         <v>42388</v>
       </c>
       <c r="B28" t="s">
@@ -2732,7 +2693,7 @@
       </c>
     </row>
     <row r="29" spans="1:7">
-      <c r="A29" s="13" t="n">
+      <c r="A29" s="7">
         <v>42388</v>
       </c>
       <c r="B29" t="s">
@@ -2755,7 +2716,7 @@
       </c>
     </row>
     <row r="30" spans="1:7">
-      <c r="A30" s="13" t="n">
+      <c r="A30" s="7">
         <v>42388</v>
       </c>
       <c r="B30" t="s">
@@ -2778,7 +2739,7 @@
       </c>
     </row>
     <row r="31" spans="1:7">
-      <c r="A31" s="13" t="n">
+      <c r="A31" s="7">
         <v>42388</v>
       </c>
       <c r="B31" t="s">
@@ -2801,7 +2762,7 @@
       </c>
     </row>
     <row r="32" spans="1:7">
-      <c r="A32" s="13" t="n">
+      <c r="A32" s="7">
         <v>42388</v>
       </c>
       <c r="B32" t="s">
@@ -2824,7 +2785,7 @@
       </c>
     </row>
     <row r="33" spans="1:7">
-      <c r="A33" s="13" t="n">
+      <c r="A33" s="7">
         <v>42388</v>
       </c>
       <c r="B33" t="s">
@@ -2847,7 +2808,7 @@
       </c>
     </row>
     <row r="34" spans="1:7">
-      <c r="A34" s="13" t="n">
+      <c r="A34" s="7">
         <v>42388</v>
       </c>
       <c r="B34" t="s">
@@ -2870,7 +2831,7 @@
       </c>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="13" t="n">
+      <c r="A35" s="7">
         <v>42388</v>
       </c>
       <c r="B35" t="s">
@@ -2893,7 +2854,7 @@
       </c>
     </row>
     <row r="36" spans="1:7">
-      <c r="A36" s="13" t="n">
+      <c r="A36" s="7">
         <v>42388</v>
       </c>
       <c r="B36" t="s">
@@ -2916,7 +2877,7 @@
       </c>
     </row>
     <row r="37" spans="1:7">
-      <c r="A37" s="13" t="n">
+      <c r="A37" s="7">
         <v>42388</v>
       </c>
       <c r="B37" t="s">
@@ -2939,7 +2900,7 @@
       </c>
     </row>
     <row r="38" spans="1:7">
-      <c r="A38" s="13" t="n">
+      <c r="A38" s="7">
         <v>42388</v>
       </c>
       <c r="B38" t="s">
@@ -2962,488 +2923,488 @@
       </c>
     </row>
     <row r="39" spans="1:7">
-      <c r="A39" s="9" t="n">
+      <c r="A39" s="3">
         <v>42388</v>
       </c>
-      <c r="B39" s="10" t="s">
+      <c r="B39" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="C39" s="10" t="n"/>
-      <c r="D39" s="10" t="s">
+      <c r="C39" s="4"/>
+      <c r="D39" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="E39" s="10" t="s">
+      <c r="E39" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="F39" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="G39" s="10" t="s">
+      <c r="F39" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G39" s="4" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="40" spans="1:7">
-      <c r="A40" s="11" t="n">
+      <c r="A40" s="5">
         <v>42387</v>
       </c>
-      <c r="B40" s="12" t="s">
+      <c r="B40" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="C40" s="12" t="n"/>
-      <c r="D40" s="12" t="s">
+      <c r="C40" s="6"/>
+      <c r="D40" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="E40" s="12" t="s">
+      <c r="E40" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="F40" s="12" t="n"/>
-      <c r="G40" s="12" t="s">
+      <c r="F40" s="6"/>
+      <c r="G40" s="6" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="41" spans="1:7">
-      <c r="A41" s="9" t="n">
+      <c r="A41" s="3">
         <v>42387</v>
       </c>
-      <c r="B41" s="10" t="s">
+      <c r="B41" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="C41" s="10" t="n"/>
-      <c r="D41" s="10" t="s">
+      <c r="C41" s="4"/>
+      <c r="D41" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="E41" s="10" t="s">
+      <c r="E41" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="F41" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="G41" s="10" t="s">
+      <c r="F41" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G41" s="4" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="42" spans="1:7">
-      <c r="A42" s="9" t="n">
+      <c r="A42" s="3">
         <v>42387</v>
       </c>
-      <c r="B42" s="10" t="s">
+      <c r="B42" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="C42" s="10" t="n"/>
-      <c r="D42" s="10" t="s">
+      <c r="C42" s="4"/>
+      <c r="D42" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="E42" s="10" t="s">
+      <c r="E42" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="F42" s="10" t="s">
+      <c r="F42" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="G42" s="10" t="s">
+      <c r="G42" s="4" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="43" spans="1:7">
-      <c r="A43" s="9" t="n">
+      <c r="A43" s="3">
         <v>42387</v>
       </c>
-      <c r="B43" s="10" t="s">
+      <c r="B43" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="C43" s="10" t="n"/>
-      <c r="D43" s="10" t="s">
+      <c r="C43" s="4"/>
+      <c r="D43" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="E43" s="10" t="s">
+      <c r="E43" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="F43" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="G43" s="10" t="s">
+      <c r="F43" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G43" s="4" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="44" spans="1:7">
-      <c r="A44" s="9" t="n">
+      <c r="A44" s="3">
         <v>42387</v>
       </c>
-      <c r="B44" s="10" t="s">
+      <c r="B44" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="C44" s="10" t="n"/>
-      <c r="D44" s="10" t="s">
+      <c r="C44" s="4"/>
+      <c r="D44" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="E44" s="10" t="s">
+      <c r="E44" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="F44" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="G44" s="10" t="s">
+      <c r="F44" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G44" s="4" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="45" spans="1:7">
-      <c r="A45" s="9" t="n">
+      <c r="A45" s="3">
         <v>42387</v>
       </c>
-      <c r="B45" s="10" t="s">
+      <c r="B45" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="C45" s="10" t="n"/>
-      <c r="D45" s="10" t="s">
+      <c r="C45" s="4"/>
+      <c r="D45" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="E45" s="10" t="s">
+      <c r="E45" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="F45" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="G45" s="10" t="s">
+      <c r="F45" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G45" s="4" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="46" spans="1:7">
-      <c r="A46" s="9" t="n">
+      <c r="A46" s="3">
         <v>42387</v>
       </c>
-      <c r="B46" s="10" t="s">
+      <c r="B46" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="C46" s="10" t="n"/>
-      <c r="D46" s="10" t="s">
+      <c r="C46" s="4"/>
+      <c r="D46" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="E46" s="10" t="s">
+      <c r="E46" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="F46" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="G46" s="10" t="s">
+      <c r="F46" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G46" s="4" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="47" spans="1:7">
-      <c r="A47" s="9" t="n">
+      <c r="A47" s="3">
         <v>42387</v>
       </c>
-      <c r="B47" s="10" t="s">
+      <c r="B47" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="C47" s="10" t="n"/>
-      <c r="D47" s="10" t="s">
+      <c r="C47" s="4"/>
+      <c r="D47" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="E47" s="10" t="s">
+      <c r="E47" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="F47" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="G47" s="10" t="s">
+      <c r="F47" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G47" s="4" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="48" spans="1:7">
-      <c r="A48" s="9" t="n">
+      <c r="A48" s="3">
         <v>42387</v>
       </c>
-      <c r="B48" s="10" t="s">
+      <c r="B48" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="C48" s="10" t="n"/>
-      <c r="D48" s="10" t="s">
+      <c r="C48" s="4"/>
+      <c r="D48" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="E48" s="10" t="s">
+      <c r="E48" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="F48" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="G48" s="10" t="s">
+      <c r="F48" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G48" s="4" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="49" spans="1:7">
-      <c r="A49" s="9" t="n">
+      <c r="A49" s="3">
         <v>42387</v>
       </c>
-      <c r="B49" s="10" t="s">
+      <c r="B49" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="C49" s="10" t="n"/>
-      <c r="D49" s="10" t="s">
+      <c r="C49" s="4"/>
+      <c r="D49" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="E49" s="10" t="s">
+      <c r="E49" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="F49" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="G49" s="10" t="s">
+      <c r="F49" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G49" s="4" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="50" spans="1:7">
-      <c r="A50" s="9" t="n">
+      <c r="A50" s="3">
         <v>42387</v>
       </c>
-      <c r="B50" s="10" t="s">
+      <c r="B50" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="C50" s="10" t="n"/>
-      <c r="D50" s="10" t="s">
+      <c r="C50" s="4"/>
+      <c r="D50" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="E50" s="10" t="s">
+      <c r="E50" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="F50" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="G50" s="10" t="s">
+      <c r="F50" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G50" s="4" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="51" spans="1:7">
-      <c r="A51" s="9" t="n">
+      <c r="A51" s="3">
         <v>42387</v>
       </c>
-      <c r="B51" s="10" t="s">
+      <c r="B51" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="C51" s="10" t="n"/>
-      <c r="D51" s="10" t="s">
+      <c r="C51" s="4"/>
+      <c r="D51" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="E51" s="10" t="s">
+      <c r="E51" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="F51" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="G51" s="10" t="s">
+      <c r="F51" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G51" s="4" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="52" spans="1:7">
-      <c r="A52" s="9" t="n">
+      <c r="A52" s="3">
         <v>42387</v>
       </c>
-      <c r="B52" s="10" t="s">
+      <c r="B52" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="C52" s="10" t="n"/>
-      <c r="D52" s="10" t="s">
+      <c r="C52" s="4"/>
+      <c r="D52" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="E52" s="10" t="s">
+      <c r="E52" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="F52" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="G52" s="10" t="s">
+      <c r="F52" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G52" s="4" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="53" spans="1:7">
-      <c r="A53" s="9" t="n">
+      <c r="A53" s="3">
         <v>42387</v>
       </c>
-      <c r="B53" s="10" t="s">
+      <c r="B53" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="C53" s="10" t="n"/>
-      <c r="D53" s="10" t="s">
+      <c r="C53" s="4"/>
+      <c r="D53" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="E53" s="10" t="s">
+      <c r="E53" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="F53" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="G53" s="10" t="s">
+      <c r="F53" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G53" s="4" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="54" spans="1:7">
-      <c r="A54" s="9" t="n">
+      <c r="A54" s="3">
         <v>42387</v>
       </c>
-      <c r="B54" s="10" t="s">
+      <c r="B54" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="C54" s="10" t="n"/>
-      <c r="D54" s="10" t="s">
+      <c r="C54" s="4"/>
+      <c r="D54" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="E54" s="10" t="s">
+      <c r="E54" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="F54" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="G54" s="10" t="s">
+      <c r="F54" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G54" s="4" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="55" spans="1:7">
-      <c r="A55" s="9" t="n">
+      <c r="A55" s="3">
         <v>42387</v>
       </c>
-      <c r="B55" s="10" t="s">
+      <c r="B55" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="C55" s="10" t="n"/>
-      <c r="D55" s="10" t="s">
+      <c r="C55" s="4"/>
+      <c r="D55" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="E55" s="10" t="s">
+      <c r="E55" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="F55" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="G55" s="10" t="s">
+      <c r="F55" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G55" s="4" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="56" spans="1:7">
-      <c r="A56" s="9" t="n">
+      <c r="A56" s="3">
         <v>42387</v>
       </c>
-      <c r="B56" s="10" t="s">
+      <c r="B56" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="C56" s="10" t="n"/>
-      <c r="D56" s="10" t="s">
+      <c r="C56" s="4"/>
+      <c r="D56" s="4" t="s">
         <v>193</v>
       </c>
-      <c r="E56" s="10" t="s">
+      <c r="E56" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="F56" s="10" t="s">
+      <c r="F56" s="4" t="s">
         <v>195</v>
       </c>
-      <c r="G56" s="10" t="s">
+      <c r="G56" s="4" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="57" spans="1:7">
-      <c r="A57" s="9" t="n">
+      <c r="A57" s="3">
         <v>42387</v>
       </c>
-      <c r="B57" s="10" t="s">
+      <c r="B57" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="C57" s="10" t="n"/>
-      <c r="D57" s="10" t="s">
+      <c r="C57" s="4"/>
+      <c r="D57" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="E57" s="10" t="s">
+      <c r="E57" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="F57" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="G57" s="10" t="s">
+      <c r="F57" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G57" s="4" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="58" spans="1:7">
-      <c r="A58" s="9" t="n">
+      <c r="A58" s="3">
         <v>42387</v>
       </c>
-      <c r="B58" s="10" t="s">
+      <c r="B58" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="C58" s="10" t="n"/>
-      <c r="D58" s="10" t="s">
+      <c r="C58" s="4"/>
+      <c r="D58" s="4" t="s">
         <v>199</v>
       </c>
-      <c r="E58" s="10" t="s">
+      <c r="E58" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="F58" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="G58" s="10" t="s">
+      <c r="F58" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G58" s="4" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="59" spans="1:7">
-      <c r="A59" s="9" t="n">
+      <c r="A59" s="3">
         <v>42387</v>
       </c>
-      <c r="B59" s="10" t="s">
+      <c r="B59" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="C59" s="10" t="n"/>
-      <c r="D59" s="10" t="s">
+      <c r="C59" s="4"/>
+      <c r="D59" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="E59" s="10" t="s">
+      <c r="E59" s="4" t="s">
         <v>203</v>
       </c>
-      <c r="F59" s="10" t="s">
+      <c r="F59" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="G59" s="10" t="s">
+      <c r="G59" s="4" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="60" spans="1:7">
-      <c r="A60" s="9" t="n">
+      <c r="A60" s="3">
         <v>42387</v>
       </c>
-      <c r="B60" s="10" t="s">
+      <c r="B60" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="C60" s="10" t="n"/>
-      <c r="D60" s="10" t="s">
+      <c r="C60" s="4"/>
+      <c r="D60" s="4" t="s">
         <v>205</v>
       </c>
-      <c r="E60" s="10" t="s">
+      <c r="E60" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="F60" s="10" t="s">
+      <c r="F60" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="G60" s="10" t="s">
+      <c r="G60" s="4" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="61" spans="1:7">
-      <c r="A61" s="9" t="n">
+      <c r="A61" s="3">
         <v>42387</v>
       </c>
-      <c r="B61" s="10" t="s">
+      <c r="B61" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="C61" s="10" t="n"/>
-      <c r="D61" s="10" t="s">
+      <c r="C61" s="4"/>
+      <c r="D61" s="4" t="s">
         <v>207</v>
       </c>
-      <c r="E61" s="10" t="s">
+      <c r="E61" s="4" t="s">
         <v>208</v>
       </c>
-      <c r="F61" s="10" t="s">
+      <c r="F61" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="G61" s="10" t="s">
+      <c r="G61" s="4" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="62" spans="1:7">
-      <c r="A62" s="13" t="n">
+      <c r="A62" s="7">
         <v>42387</v>
       </c>
       <c r="B62" t="s">
@@ -3466,7 +3427,7 @@
       </c>
     </row>
     <row r="63" spans="1:7">
-      <c r="A63" s="13" t="n">
+      <c r="A63" s="7">
         <v>42387</v>
       </c>
       <c r="B63" t="s">
@@ -3489,7 +3450,7 @@
       </c>
     </row>
     <row r="64" spans="1:7">
-      <c r="A64" s="13" t="n">
+      <c r="A64" s="7">
         <v>42387</v>
       </c>
       <c r="B64" t="s">
@@ -3512,28 +3473,28 @@
       </c>
     </row>
     <row r="65" spans="1:7">
-      <c r="A65" s="9" t="n">
+      <c r="A65" s="3">
         <v>42387</v>
       </c>
-      <c r="B65" s="10" t="s">
+      <c r="B65" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="C65" s="10" t="n"/>
-      <c r="D65" s="10" t="s">
+      <c r="C65" s="4"/>
+      <c r="D65" s="4" t="s">
         <v>217</v>
       </c>
-      <c r="E65" s="10" t="s">
+      <c r="E65" s="4" t="s">
         <v>218</v>
       </c>
-      <c r="F65" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="G65" s="10" t="s">
+      <c r="F65" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G65" s="4" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="66" spans="1:7">
-      <c r="A66" s="13" t="n">
+      <c r="A66" s="7">
         <v>42384</v>
       </c>
       <c r="B66" t="s">
@@ -3556,7 +3517,7 @@
       </c>
     </row>
     <row r="67" spans="1:7">
-      <c r="A67" s="13" t="n">
+      <c r="A67" s="7">
         <v>42384</v>
       </c>
       <c r="B67" t="s">
@@ -3579,7 +3540,7 @@
       </c>
     </row>
     <row r="68" spans="1:7">
-      <c r="A68" s="13" t="n">
+      <c r="A68" s="7">
         <v>42384</v>
       </c>
       <c r="B68" t="s">
@@ -3602,7 +3563,7 @@
       </c>
     </row>
     <row r="69" spans="1:7">
-      <c r="A69" s="13" t="n">
+      <c r="A69" s="7">
         <v>42384</v>
       </c>
       <c r="B69" t="s">
@@ -3625,7 +3586,7 @@
       </c>
     </row>
     <row r="70" spans="1:7">
-      <c r="A70" s="13" t="n">
+      <c r="A70" s="7">
         <v>42384</v>
       </c>
       <c r="B70" t="s">
@@ -3648,64 +3609,64 @@
       </c>
     </row>
     <row r="71" spans="1:7">
-      <c r="A71" s="11" t="n">
+      <c r="A71" s="5">
         <v>42384</v>
       </c>
-      <c r="B71" s="12" t="s">
+      <c r="B71" s="6" t="s">
         <v>233</v>
       </c>
-      <c r="C71" s="12" t="n"/>
-      <c r="D71" s="12" t="s">
+      <c r="C71" s="6"/>
+      <c r="D71" s="6" t="s">
         <v>234</v>
       </c>
-      <c r="E71" s="12" t="s">
+      <c r="E71" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="F71" s="12" t="n"/>
-      <c r="G71" s="12" t="s">
+      <c r="F71" s="6"/>
+      <c r="G71" s="6" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="72" spans="1:7">
-      <c r="A72" s="11" t="n">
+      <c r="A72" s="5">
         <v>42384</v>
       </c>
-      <c r="B72" s="12" t="s">
+      <c r="B72" s="6" t="s">
         <v>235</v>
       </c>
-      <c r="C72" s="12" t="n"/>
-      <c r="D72" s="12" t="s">
+      <c r="C72" s="6"/>
+      <c r="D72" s="6" t="s">
         <v>236</v>
       </c>
-      <c r="E72" s="12" t="s">
+      <c r="E72" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="F72" s="12" t="n"/>
-      <c r="G72" s="12" t="s">
+      <c r="F72" s="6"/>
+      <c r="G72" s="6" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="73" spans="1:7">
-      <c r="A73" s="11" t="n">
+      <c r="A73" s="5">
         <v>42384</v>
       </c>
-      <c r="B73" s="12" t="s">
+      <c r="B73" s="6" t="s">
         <v>238</v>
       </c>
-      <c r="C73" s="12" t="n"/>
-      <c r="D73" s="12" t="s">
+      <c r="C73" s="6"/>
+      <c r="D73" s="6" t="s">
         <v>239</v>
       </c>
-      <c r="E73" s="12" t="s">
+      <c r="E73" s="6" t="s">
         <v>240</v>
       </c>
-      <c r="F73" s="12" t="n"/>
-      <c r="G73" s="12" t="s">
+      <c r="F73" s="6"/>
+      <c r="G73" s="6" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="74" spans="1:7">
-      <c r="A74" s="13" t="n">
+      <c r="A74" s="7">
         <v>42384</v>
       </c>
       <c r="B74" t="s">
@@ -3728,7 +3689,7 @@
       </c>
     </row>
     <row r="75" spans="1:7">
-      <c r="A75" s="13" t="n">
+      <c r="A75" s="7">
         <v>42384</v>
       </c>
       <c r="B75" t="s">
@@ -3751,7 +3712,7 @@
       </c>
     </row>
     <row r="76" spans="1:7">
-      <c r="A76" s="13" t="n">
+      <c r="A76" s="7">
         <v>42384</v>
       </c>
       <c r="B76" t="s">
@@ -3774,26 +3735,26 @@
       </c>
     </row>
     <row r="77" spans="1:7">
-      <c r="A77" s="11" t="n">
+      <c r="A77" s="5">
         <v>42384</v>
       </c>
-      <c r="B77" s="12" t="s">
+      <c r="B77" s="6" t="s">
         <v>247</v>
       </c>
-      <c r="C77" s="12" t="n"/>
-      <c r="D77" s="12" t="s">
+      <c r="C77" s="6"/>
+      <c r="D77" s="6" t="s">
         <v>248</v>
       </c>
-      <c r="E77" s="12" t="s">
+      <c r="E77" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="F77" s="12" t="n"/>
-      <c r="G77" s="12" t="s">
+      <c r="F77" s="6"/>
+      <c r="G77" s="6" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="78" spans="1:7">
-      <c r="A78" s="13" t="n">
+      <c r="A78" s="7">
         <v>42384</v>
       </c>
       <c r="B78" t="s">
@@ -3816,7 +3777,7 @@
       </c>
     </row>
     <row r="79" spans="1:7">
-      <c r="A79" s="13" t="n">
+      <c r="A79" s="7">
         <v>42384</v>
       </c>
       <c r="B79" t="s">
@@ -3839,7 +3800,7 @@
       </c>
     </row>
     <row r="80" spans="1:7">
-      <c r="A80" s="13" t="n">
+      <c r="A80" s="7">
         <v>42383</v>
       </c>
       <c r="B80" t="s">
@@ -3862,7 +3823,7 @@
       </c>
     </row>
     <row r="81" spans="1:7">
-      <c r="A81" s="13" t="n">
+      <c r="A81" s="7">
         <v>42383</v>
       </c>
       <c r="B81" t="s">
@@ -3885,7 +3846,7 @@
       </c>
     </row>
     <row r="82" spans="1:7">
-      <c r="A82" s="13" t="n">
+      <c r="A82" s="7">
         <v>42383</v>
       </c>
       <c r="B82" t="s">
@@ -3908,7 +3869,7 @@
       </c>
     </row>
     <row r="83" spans="1:7">
-      <c r="A83" s="13" t="n">
+      <c r="A83" s="7">
         <v>42383</v>
       </c>
       <c r="B83" t="s">
@@ -3931,44 +3892,39 @@
       </c>
     </row>
     <row r="84" spans="1:7">
-      <c r="A84" s="9" t="n">
+      <c r="A84" s="3">
         <v>42383</v>
       </c>
-      <c r="B84" s="10" t="s">
+      <c r="B84" s="4" t="s">
         <v>266</v>
       </c>
-      <c r="C84" s="10" t="n"/>
-      <c r="D84" s="10" t="s">
+      <c r="C84" s="4"/>
+      <c r="D84" s="4" t="s">
         <v>267</v>
       </c>
-      <c r="E84" s="10" t="s">
+      <c r="E84" s="4" t="s">
         <v>268</v>
       </c>
-      <c r="F84" s="10" t="s">
+      <c r="F84" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="G84" s="10" t="s">
+      <c r="G84" s="4" t="s">
         <v>51</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G94"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="16.5"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
@@ -3994,102 +3950,102 @@
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="11" t="n">
+      <c r="A2" s="5">
         <v>42395</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="6" t="s">
         <v>269</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="6" t="s">
         <v>270</v>
       </c>
-      <c r="E2" s="12" t="s"/>
-      <c r="F2" s="12" t="s"/>
-      <c r="G2" s="12" t="s">
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="14" t="n">
+      <c r="A3" s="8">
         <v>42395</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="9" t="s">
         <v>272</v>
       </c>
-      <c r="E3" s="15" t="s"/>
-      <c r="F3" s="15" t="s"/>
-      <c r="G3" s="15" t="s">
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="9" t="n">
+      <c r="A4" s="3">
         <v>42395</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="4" t="s">
         <v>273</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="4" t="s">
         <v>274</v>
       </c>
-      <c r="E4" s="10" t="s"/>
-      <c r="F4" s="10" t="s"/>
-      <c r="G4" s="10" t="s">
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="9" t="n">
+      <c r="A5" s="3">
         <v>42394</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="4" t="s">
         <v>275</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="4" t="s">
         <v>276</v>
       </c>
-      <c r="E5" s="10" t="s"/>
-      <c r="F5" s="10" t="s"/>
-      <c r="G5" s="10" t="s">
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="14" t="n">
+      <c r="A6" s="8">
         <v>42394</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="9" t="s">
         <v>277</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="15" t="s">
+      <c r="D6" s="9" t="s">
         <v>278</v>
       </c>
-      <c r="E6" s="15" t="s"/>
-      <c r="F6" s="15" t="s"/>
-      <c r="G6" s="15" t="s">
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="13" t="n">
+      <c r="A7" s="7">
         <v>42394</v>
       </c>
       <c r="B7" t="s">
@@ -4112,7 +4068,7 @@
       </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="13" t="n">
+      <c r="A8" s="7">
         <v>42394</v>
       </c>
       <c r="B8" t="s">
@@ -4135,220 +4091,220 @@
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="14" t="n">
+      <c r="A9" s="8">
         <v>42390</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="9" t="s">
         <v>285</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="15" t="s">
+      <c r="D9" s="9" t="s">
         <v>286</v>
       </c>
-      <c r="E9" s="15" t="s"/>
-      <c r="F9" s="15" t="s"/>
-      <c r="G9" s="15" t="s">
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="9" t="n">
+      <c r="A10" s="3">
         <v>42390</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="4" t="s">
         <v>287</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="D10" s="4" t="s">
         <v>288</v>
       </c>
-      <c r="E10" s="10" t="s"/>
-      <c r="F10" s="10" t="s"/>
-      <c r="G10" s="10" t="s">
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="9" t="n">
+      <c r="A11" s="3">
         <v>42395</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="4" t="s">
         <v>289</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="D11" s="4" t="s">
         <v>290</v>
       </c>
-      <c r="E11" s="10" t="s"/>
-      <c r="F11" s="10" t="s"/>
-      <c r="G11" s="10" t="s">
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="9" t="n">
+      <c r="A12" s="3">
         <v>42395</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="4" t="s">
         <v>291</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C12" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="D12" s="4" t="s">
         <v>292</v>
       </c>
-      <c r="E12" s="10" t="s"/>
-      <c r="F12" s="10" t="s"/>
-      <c r="G12" s="10" t="s">
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="11" t="n">
+      <c r="A13" s="5">
         <v>42395</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="6" t="s">
         <v>293</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C13" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="D13" s="12" t="s">
+      <c r="D13" s="6" t="s">
         <v>294</v>
       </c>
-      <c r="E13" s="12" t="s"/>
-      <c r="F13" s="12" t="s"/>
-      <c r="G13" s="12" t="s">
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="11" t="n">
+      <c r="A14" s="5">
         <v>42395</v>
       </c>
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="6" t="s">
         <v>295</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="C14" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="D14" s="12" t="s">
+      <c r="D14" s="6" t="s">
         <v>296</v>
       </c>
-      <c r="E14" s="12" t="s"/>
-      <c r="F14" s="12" t="s"/>
-      <c r="G14" s="12" t="s">
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="11" t="n">
+      <c r="A15" s="5">
         <v>42395</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="6" t="s">
         <v>297</v>
       </c>
-      <c r="C15" s="12" t="s">
+      <c r="C15" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="D15" s="12" t="s">
+      <c r="D15" s="6" t="s">
         <v>298</v>
       </c>
-      <c r="E15" s="12" t="s"/>
-      <c r="F15" s="12" t="s"/>
-      <c r="G15" s="12" t="s">
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="11" t="n">
+      <c r="A16" s="5">
         <v>42395</v>
       </c>
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="6" t="s">
         <v>299</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="C16" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="D16" s="12" t="s">
+      <c r="D16" s="6" t="s">
         <v>300</v>
       </c>
-      <c r="E16" s="12" t="s"/>
-      <c r="F16" s="12" t="s"/>
-      <c r="G16" s="12" t="s">
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="11" t="n">
+      <c r="A17" s="5">
         <v>42395</v>
       </c>
-      <c r="B17" s="12" t="s">
+      <c r="B17" s="6" t="s">
         <v>301</v>
       </c>
-      <c r="C17" s="12" t="s">
+      <c r="C17" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="D17" s="12" t="s">
+      <c r="D17" s="6" t="s">
         <v>302</v>
       </c>
-      <c r="E17" s="12" t="s"/>
-      <c r="F17" s="12" t="s"/>
-      <c r="G17" s="12" t="s">
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="9" t="n">
+      <c r="A18" s="3">
         <v>42395</v>
       </c>
-      <c r="B18" s="10" t="s">
+      <c r="B18" s="4" t="s">
         <v>303</v>
       </c>
-      <c r="C18" s="10" t="s">
+      <c r="C18" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D18" s="10" t="s">
+      <c r="D18" s="4" t="s">
         <v>304</v>
       </c>
-      <c r="E18" s="10" t="s"/>
-      <c r="F18" s="10" t="s"/>
-      <c r="G18" s="10" t="s">
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="9" t="n">
+      <c r="A19" s="3">
         <v>42394</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="B19" s="4" t="s">
         <v>305</v>
       </c>
-      <c r="C19" s="10" t="s">
+      <c r="C19" s="4" t="s">
         <v>306</v>
       </c>
-      <c r="D19" s="10" t="s">
+      <c r="D19" s="4" t="s">
         <v>307</v>
       </c>
-      <c r="E19" s="10" t="s">
+      <c r="E19" s="4" t="s">
         <v>308</v>
       </c>
-      <c r="F19" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="G19" s="10" t="s">
+      <c r="F19" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G19" s="4" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" s="13" t="n">
+      <c r="A20" s="7">
         <v>42394</v>
       </c>
       <c r="B20" t="s">
@@ -4371,24 +4327,24 @@
       </c>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="9" t="n">
+      <c r="A21" s="3">
         <v>42396</v>
       </c>
-      <c r="B21" s="10" t="s">
+      <c r="B21" s="4" t="s">
         <v>312</v>
       </c>
-      <c r="C21" s="10" t="s"/>
-      <c r="D21" s="10" t="s">
+      <c r="C21" s="4"/>
+      <c r="D21" s="4" t="s">
         <v>313</v>
       </c>
-      <c r="E21" s="10" t="s"/>
-      <c r="F21" s="10" t="s"/>
-      <c r="G21" s="10" t="s">
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:7">
-      <c r="A22" s="13" t="n">
+      <c r="A22" s="7">
         <v>42395</v>
       </c>
       <c r="B22" t="s">
@@ -4411,143 +4367,143 @@
       </c>
     </row>
     <row r="23" spans="1:7">
-      <c r="A23" s="11" t="n">
+      <c r="A23" s="5">
         <v>42394</v>
       </c>
-      <c r="B23" s="12" t="s">
+      <c r="B23" s="6" t="s">
         <v>317</v>
       </c>
-      <c r="C23" s="12" t="s"/>
-      <c r="D23" s="12" t="s">
+      <c r="C23" s="6"/>
+      <c r="D23" s="6" t="s">
         <v>318</v>
       </c>
-      <c r="E23" s="12" t="s"/>
-      <c r="F23" s="12" t="s"/>
-      <c r="G23" s="12" t="s">
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="24" spans="1:7">
-      <c r="A24" s="9" t="n">
+      <c r="A24" s="3">
         <v>42390</v>
       </c>
-      <c r="B24" s="10" t="s">
+      <c r="B24" s="4" t="s">
         <v>319</v>
       </c>
-      <c r="C24" s="10" t="s"/>
-      <c r="D24" s="10" t="s">
+      <c r="C24" s="4"/>
+      <c r="D24" s="4" t="s">
         <v>320</v>
       </c>
-      <c r="E24" s="10" t="s"/>
-      <c r="F24" s="10" t="s"/>
-      <c r="G24" s="10" t="s">
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="25" spans="1:7">
-      <c r="A25" s="11" t="n">
+      <c r="A25" s="5">
         <v>42390</v>
       </c>
-      <c r="B25" s="12" t="s">
+      <c r="B25" s="6" t="s">
         <v>321</v>
       </c>
-      <c r="C25" s="12" t="s"/>
-      <c r="D25" s="12" t="s">
+      <c r="C25" s="6"/>
+      <c r="D25" s="6" t="s">
         <v>322</v>
       </c>
-      <c r="E25" s="12" t="s"/>
-      <c r="F25" s="12" t="s"/>
-      <c r="G25" s="12" t="s">
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="26" spans="1:7">
-      <c r="A26" s="9" t="n">
+      <c r="A26" s="3">
         <v>42396</v>
       </c>
-      <c r="B26" s="10" t="s">
+      <c r="B26" s="4" t="s">
         <v>323</v>
       </c>
-      <c r="C26" s="10" t="s"/>
-      <c r="D26" s="10" t="s">
+      <c r="C26" s="4"/>
+      <c r="D26" s="4" t="s">
         <v>324</v>
       </c>
-      <c r="E26" s="10" t="s"/>
-      <c r="F26" s="10" t="s"/>
-      <c r="G26" s="10" t="s">
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="27" spans="1:7">
-      <c r="A27" s="9" t="n">
+      <c r="A27" s="3">
         <v>42396</v>
       </c>
-      <c r="B27" s="10" t="s">
+      <c r="B27" s="4" t="s">
         <v>325</v>
       </c>
-      <c r="C27" s="10" t="s"/>
-      <c r="D27" s="10" t="s">
+      <c r="C27" s="4"/>
+      <c r="D27" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="E27" s="10" t="s"/>
-      <c r="F27" s="10" t="s"/>
-      <c r="G27" s="10" t="s">
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="28" spans="1:7">
-      <c r="A28" s="9" t="n">
+      <c r="A28" s="3">
         <v>42396</v>
       </c>
-      <c r="B28" s="10" t="s">
+      <c r="B28" s="4" t="s">
         <v>327</v>
       </c>
-      <c r="C28" s="10" t="s"/>
-      <c r="D28" s="10" t="s">
+      <c r="C28" s="4"/>
+      <c r="D28" s="4" t="s">
         <v>328</v>
       </c>
-      <c r="E28" s="10" t="s"/>
-      <c r="F28" s="10" t="s"/>
-      <c r="G28" s="10" t="s">
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="29" spans="1:7">
-      <c r="A29" s="9" t="n">
+      <c r="A29" s="3">
         <v>42396</v>
       </c>
-      <c r="B29" s="10" t="s">
+      <c r="B29" s="4" t="s">
         <v>329</v>
       </c>
-      <c r="C29" s="10" t="s"/>
-      <c r="D29" s="10" t="s">
+      <c r="C29" s="4"/>
+      <c r="D29" s="4" t="s">
         <v>330</v>
       </c>
-      <c r="E29" s="10" t="s"/>
-      <c r="F29" s="10" t="s"/>
-      <c r="G29" s="10" t="s">
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="30" spans="1:7">
-      <c r="A30" s="9" t="n">
+      <c r="A30" s="3">
         <v>42396</v>
       </c>
-      <c r="B30" s="10" t="s">
+      <c r="B30" s="4" t="s">
         <v>331</v>
       </c>
-      <c r="C30" s="10" t="s"/>
-      <c r="D30" s="10" t="s">
+      <c r="C30" s="4"/>
+      <c r="D30" s="4" t="s">
         <v>332</v>
       </c>
-      <c r="E30" s="10" t="s"/>
-      <c r="F30" s="10" t="s"/>
-      <c r="G30" s="10" t="s">
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="31" spans="1:7">
-      <c r="A31" s="13" t="n">
+      <c r="A31" s="7">
         <v>42396</v>
       </c>
       <c r="B31" t="s">
@@ -4570,7 +4526,7 @@
       </c>
     </row>
     <row r="32" spans="1:7">
-      <c r="A32" s="13" t="n">
+      <c r="A32" s="7">
         <v>42396</v>
       </c>
       <c r="B32" t="s">
@@ -4593,233 +4549,233 @@
       </c>
     </row>
     <row r="33" spans="1:7">
-      <c r="A33" s="9" t="n">
+      <c r="A33" s="3">
         <v>42396</v>
       </c>
-      <c r="B33" s="10" t="s">
+      <c r="B33" s="4" t="s">
         <v>339</v>
       </c>
-      <c r="C33" s="10" t="s"/>
-      <c r="D33" s="10" t="s">
+      <c r="C33" s="4"/>
+      <c r="D33" s="4" t="s">
         <v>340</v>
       </c>
-      <c r="E33" s="10" t="s"/>
-      <c r="F33" s="10" t="s"/>
-      <c r="G33" s="10" t="s">
+      <c r="E33" s="4"/>
+      <c r="F33" s="4"/>
+      <c r="G33" s="4" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="34" spans="1:7">
-      <c r="A34" s="11" t="n">
+      <c r="A34" s="5">
         <v>42395</v>
       </c>
-      <c r="B34" s="12" t="s">
+      <c r="B34" s="6" t="s">
         <v>341</v>
       </c>
-      <c r="C34" s="12" t="s"/>
-      <c r="D34" s="12" t="s">
+      <c r="C34" s="6"/>
+      <c r="D34" s="6" t="s">
         <v>342</v>
       </c>
-      <c r="E34" s="12" t="s">
+      <c r="E34" s="6" t="s">
         <v>343</v>
       </c>
-      <c r="F34" s="12" t="s"/>
-      <c r="G34" s="12" t="s">
+      <c r="F34" s="6"/>
+      <c r="G34" s="6" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="11" t="n">
+      <c r="A35" s="5">
         <v>42395</v>
       </c>
-      <c r="B35" s="12" t="s">
+      <c r="B35" s="6" t="s">
         <v>344</v>
       </c>
-      <c r="C35" s="12" t="s"/>
-      <c r="D35" s="12" t="s">
+      <c r="C35" s="6"/>
+      <c r="D35" s="6" t="s">
         <v>345</v>
       </c>
-      <c r="E35" s="12" t="s">
+      <c r="E35" s="6" t="s">
         <v>346</v>
       </c>
-      <c r="F35" s="12" t="s"/>
-      <c r="G35" s="12" t="s">
+      <c r="F35" s="6"/>
+      <c r="G35" s="6" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="36" spans="1:7">
-      <c r="A36" s="11" t="n">
+      <c r="A36" s="5">
         <v>42395</v>
       </c>
-      <c r="B36" s="12" t="s">
+      <c r="B36" s="6" t="s">
         <v>347</v>
       </c>
-      <c r="C36" s="12" t="s"/>
-      <c r="D36" s="12" t="s">
+      <c r="C36" s="6"/>
+      <c r="D36" s="6" t="s">
         <v>348</v>
       </c>
-      <c r="E36" s="12" t="s">
+      <c r="E36" s="6" t="s">
         <v>349</v>
       </c>
-      <c r="F36" s="12" t="s"/>
-      <c r="G36" s="12" t="s">
+      <c r="F36" s="6"/>
+      <c r="G36" s="6" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="37" spans="1:7">
-      <c r="A37" s="11" t="n">
+      <c r="A37" s="5">
         <v>42395</v>
       </c>
-      <c r="B37" s="12" t="s">
+      <c r="B37" s="6" t="s">
         <v>350</v>
       </c>
-      <c r="C37" s="12" t="s"/>
-      <c r="D37" s="12" t="s">
+      <c r="C37" s="6"/>
+      <c r="D37" s="6" t="s">
         <v>351</v>
       </c>
-      <c r="E37" s="12" t="s">
+      <c r="E37" s="6" t="s">
         <v>352</v>
       </c>
-      <c r="F37" s="12" t="s"/>
-      <c r="G37" s="12" t="s">
+      <c r="F37" s="6"/>
+      <c r="G37" s="6" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="38" spans="1:7">
-      <c r="A38" s="11" t="n">
+      <c r="A38" s="5">
         <v>42395</v>
       </c>
-      <c r="B38" s="12" t="s">
+      <c r="B38" s="6" t="s">
         <v>353</v>
       </c>
-      <c r="C38" s="12" t="s"/>
-      <c r="D38" s="12" t="s">
+      <c r="C38" s="6"/>
+      <c r="D38" s="6" t="s">
         <v>354</v>
       </c>
-      <c r="E38" s="12" t="s">
+      <c r="E38" s="6" t="s">
         <v>355</v>
       </c>
-      <c r="F38" s="12" t="s"/>
-      <c r="G38" s="12" t="s">
+      <c r="F38" s="6"/>
+      <c r="G38" s="6" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="39" spans="1:7">
-      <c r="A39" s="11" t="n">
+      <c r="A39" s="5">
         <v>42395</v>
       </c>
-      <c r="B39" s="12" t="s">
+      <c r="B39" s="6" t="s">
         <v>356</v>
       </c>
-      <c r="C39" s="12" t="s"/>
-      <c r="D39" s="12" t="s">
+      <c r="C39" s="6"/>
+      <c r="D39" s="6" t="s">
         <v>357</v>
       </c>
-      <c r="E39" s="12" t="s">
+      <c r="E39" s="6" t="s">
         <v>358</v>
       </c>
-      <c r="F39" s="12" t="s"/>
-      <c r="G39" s="12" t="s">
+      <c r="F39" s="6"/>
+      <c r="G39" s="6" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="40" spans="1:7">
-      <c r="A40" s="11" t="n">
+      <c r="A40" s="5">
         <v>42395</v>
       </c>
-      <c r="B40" s="12" t="s">
+      <c r="B40" s="6" t="s">
         <v>359</v>
       </c>
-      <c r="C40" s="12" t="s"/>
-      <c r="D40" s="12" t="s">
+      <c r="C40" s="6"/>
+      <c r="D40" s="6" t="s">
         <v>360</v>
       </c>
-      <c r="E40" s="12" t="s">
+      <c r="E40" s="6" t="s">
         <v>361</v>
       </c>
-      <c r="F40" s="12" t="s"/>
-      <c r="G40" s="12" t="s">
+      <c r="F40" s="6"/>
+      <c r="G40" s="6" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="41" spans="1:7">
-      <c r="A41" s="11" t="n">
+      <c r="A41" s="5">
         <v>42395</v>
       </c>
-      <c r="B41" s="12" t="s">
+      <c r="B41" s="6" t="s">
         <v>362</v>
       </c>
-      <c r="C41" s="12" t="s"/>
-      <c r="D41" s="12" t="s">
+      <c r="C41" s="6"/>
+      <c r="D41" s="6" t="s">
         <v>363</v>
       </c>
-      <c r="E41" s="12" t="s">
+      <c r="E41" s="6" t="s">
         <v>364</v>
       </c>
-      <c r="F41" s="12" t="s"/>
-      <c r="G41" s="12" t="s">
+      <c r="F41" s="6"/>
+      <c r="G41" s="6" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="42" spans="1:7">
-      <c r="A42" s="11" t="n">
+      <c r="A42" s="5">
         <v>42395</v>
       </c>
-      <c r="B42" s="12" t="s">
+      <c r="B42" s="6" t="s">
         <v>365</v>
       </c>
-      <c r="C42" s="12" t="s"/>
-      <c r="D42" s="12" t="s">
+      <c r="C42" s="6"/>
+      <c r="D42" s="6" t="s">
         <v>366</v>
       </c>
-      <c r="E42" s="12" t="s">
+      <c r="E42" s="6" t="s">
         <v>367</v>
       </c>
-      <c r="F42" s="12" t="s"/>
-      <c r="G42" s="12" t="s">
+      <c r="F42" s="6"/>
+      <c r="G42" s="6" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="43" spans="1:7">
-      <c r="A43" s="11" t="n">
+      <c r="A43" s="5">
         <v>42395</v>
       </c>
-      <c r="B43" s="12" t="s">
+      <c r="B43" s="6" t="s">
         <v>368</v>
       </c>
-      <c r="C43" s="12" t="s"/>
-      <c r="D43" s="12" t="s">
+      <c r="C43" s="6"/>
+      <c r="D43" s="6" t="s">
         <v>369</v>
       </c>
-      <c r="E43" s="12" t="s">
+      <c r="E43" s="6" t="s">
         <v>370</v>
       </c>
-      <c r="F43" s="12" t="s"/>
-      <c r="G43" s="12" t="s">
+      <c r="F43" s="6"/>
+      <c r="G43" s="6" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="44" spans="1:7">
-      <c r="A44" s="11" t="n">
+      <c r="A44" s="5">
         <v>42395</v>
       </c>
-      <c r="B44" s="12" t="s">
+      <c r="B44" s="6" t="s">
         <v>371</v>
       </c>
-      <c r="C44" s="12" t="s"/>
-      <c r="D44" s="12" t="s">
+      <c r="C44" s="6"/>
+      <c r="D44" s="6" t="s">
         <v>372</v>
       </c>
-      <c r="E44" s="12" t="s">
+      <c r="E44" s="6" t="s">
         <v>373</v>
       </c>
-      <c r="F44" s="12" t="s"/>
-      <c r="G44" s="12" t="s">
+      <c r="F44" s="6"/>
+      <c r="G44" s="6" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="45" spans="1:7">
-      <c r="A45" s="13" t="n">
+      <c r="A45" s="7">
         <v>42394</v>
       </c>
       <c r="B45" t="s">
@@ -4842,7 +4798,7 @@
       </c>
     </row>
     <row r="46" spans="1:7">
-      <c r="A46" s="13" t="n">
+      <c r="A46" s="7">
         <v>42394</v>
       </c>
       <c r="B46" t="s">
@@ -4865,7 +4821,7 @@
       </c>
     </row>
     <row r="47" spans="1:7">
-      <c r="A47" s="13" t="n">
+      <c r="A47" s="7">
         <v>42394</v>
       </c>
       <c r="B47" t="s">
@@ -4888,28 +4844,28 @@
       </c>
     </row>
     <row r="48" spans="1:7">
-      <c r="A48" s="9" t="n">
+      <c r="A48" s="3">
         <v>42394</v>
       </c>
-      <c r="B48" s="10" t="s">
+      <c r="B48" s="4" t="s">
         <v>381</v>
       </c>
-      <c r="C48" s="10" t="s"/>
-      <c r="D48" s="10" t="s">
+      <c r="C48" s="4"/>
+      <c r="D48" s="4" t="s">
         <v>382</v>
       </c>
-      <c r="E48" s="10" t="s">
+      <c r="E48" s="4" t="s">
         <v>383</v>
       </c>
-      <c r="F48" s="10" t="s">
+      <c r="F48" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="G48" s="10" t="s">
+      <c r="G48" s="4" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="49" spans="1:7">
-      <c r="A49" s="13" t="n">
+      <c r="A49" s="7">
         <v>42394</v>
       </c>
       <c r="B49" t="s">
@@ -4932,28 +4888,28 @@
       </c>
     </row>
     <row r="50" spans="1:7">
-      <c r="A50" s="9" t="n">
+      <c r="A50" s="3">
         <v>42391</v>
       </c>
-      <c r="B50" s="10" t="s">
+      <c r="B50" s="4" t="s">
         <v>387</v>
       </c>
-      <c r="C50" s="10" t="s"/>
-      <c r="D50" s="10" t="s">
+      <c r="C50" s="4"/>
+      <c r="D50" s="4" t="s">
         <v>388</v>
       </c>
-      <c r="E50" s="10" t="s">
+      <c r="E50" s="4" t="s">
         <v>389</v>
       </c>
-      <c r="F50" s="10" t="s">
+      <c r="F50" s="4" t="s">
         <v>227</v>
       </c>
-      <c r="G50" s="10" t="s">
+      <c r="G50" s="4" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="51" spans="1:7">
-      <c r="A51" s="13" t="n">
+      <c r="A51" s="7">
         <v>42390</v>
       </c>
       <c r="B51" t="s">
@@ -4976,7 +4932,7 @@
       </c>
     </row>
     <row r="52" spans="1:7">
-      <c r="A52" s="13" t="n">
+      <c r="A52" s="7">
         <v>42390</v>
       </c>
       <c r="B52" t="s">
@@ -4999,7 +4955,7 @@
       </c>
     </row>
     <row r="53" spans="1:7">
-      <c r="A53" s="13" t="n">
+      <c r="A53" s="7">
         <v>42390</v>
       </c>
       <c r="B53" t="s">
@@ -5022,7 +4978,7 @@
       </c>
     </row>
     <row r="54" spans="1:7">
-      <c r="A54" s="13" t="n">
+      <c r="A54" s="7">
         <v>42390</v>
       </c>
       <c r="B54" t="s">
@@ -5045,7 +5001,7 @@
       </c>
     </row>
     <row r="55" spans="1:7">
-      <c r="A55" s="13" t="n">
+      <c r="A55" s="7">
         <v>42390</v>
       </c>
       <c r="B55" t="s">
@@ -5068,7 +5024,7 @@
       </c>
     </row>
     <row r="56" spans="1:7">
-      <c r="A56" s="13" t="n">
+      <c r="A56" s="7">
         <v>42390</v>
       </c>
       <c r="B56" t="s">
@@ -5091,7 +5047,7 @@
       </c>
     </row>
     <row r="57" spans="1:7">
-      <c r="A57" s="13" t="n">
+      <c r="A57" s="7">
         <v>42390</v>
       </c>
       <c r="B57" t="s">
@@ -5114,7 +5070,7 @@
       </c>
     </row>
     <row r="58" spans="1:7">
-      <c r="A58" s="13" t="n">
+      <c r="A58" s="7">
         <v>42390</v>
       </c>
       <c r="B58" t="s">
@@ -5137,7 +5093,7 @@
       </c>
     </row>
     <row r="59" spans="1:7">
-      <c r="A59" s="13" t="n">
+      <c r="A59" s="7">
         <v>42390</v>
       </c>
       <c r="B59" t="s">
@@ -5160,7 +5116,7 @@
       </c>
     </row>
     <row r="60" spans="1:7">
-      <c r="A60" s="13" t="n">
+      <c r="A60" s="7">
         <v>42390</v>
       </c>
       <c r="B60" t="s">
@@ -5183,7 +5139,7 @@
       </c>
     </row>
     <row r="61" spans="1:7">
-      <c r="A61" s="13" t="n">
+      <c r="A61" s="7">
         <v>42390</v>
       </c>
       <c r="B61" t="s">
@@ -5206,7 +5162,7 @@
       </c>
     </row>
     <row r="62" spans="1:7">
-      <c r="A62" s="13" t="n">
+      <c r="A62" s="7">
         <v>42390</v>
       </c>
       <c r="B62" t="s">
@@ -5229,7 +5185,7 @@
       </c>
     </row>
     <row r="63" spans="1:7">
-      <c r="A63" s="13" t="n">
+      <c r="A63" s="7">
         <v>42390</v>
       </c>
       <c r="B63" t="s">
@@ -5252,7 +5208,7 @@
       </c>
     </row>
     <row r="64" spans="1:7">
-      <c r="A64" s="13" t="n">
+      <c r="A64" s="7">
         <v>42390</v>
       </c>
       <c r="B64" t="s">
@@ -5275,7 +5231,7 @@
       </c>
     </row>
     <row r="65" spans="1:7">
-      <c r="A65" s="13" t="n">
+      <c r="A65" s="7">
         <v>42390</v>
       </c>
       <c r="B65" t="s">
@@ -5298,7 +5254,7 @@
       </c>
     </row>
     <row r="66" spans="1:7">
-      <c r="A66" s="13" t="n">
+      <c r="A66" s="7">
         <v>42390</v>
       </c>
       <c r="B66" t="s">
@@ -5321,7 +5277,7 @@
       </c>
     </row>
     <row r="67" spans="1:7">
-      <c r="A67" s="13" t="n">
+      <c r="A67" s="7">
         <v>42390</v>
       </c>
       <c r="B67" t="s">
@@ -5344,7 +5300,7 @@
       </c>
     </row>
     <row r="68" spans="1:7">
-      <c r="A68" s="13" t="n">
+      <c r="A68" s="7">
         <v>42390</v>
       </c>
       <c r="B68" t="s">
@@ -5367,7 +5323,7 @@
       </c>
     </row>
     <row r="69" spans="1:7">
-      <c r="A69" s="13" t="n">
+      <c r="A69" s="7">
         <v>42390</v>
       </c>
       <c r="B69" t="s">
@@ -5390,7 +5346,7 @@
       </c>
     </row>
     <row r="70" spans="1:7">
-      <c r="A70" s="13" t="n">
+      <c r="A70" s="7">
         <v>42390</v>
       </c>
       <c r="B70" t="s">
@@ -5413,7 +5369,7 @@
       </c>
     </row>
     <row r="71" spans="1:7">
-      <c r="A71" s="13" t="n">
+      <c r="A71" s="7">
         <v>42390</v>
       </c>
       <c r="B71" t="s">
@@ -5436,7 +5392,7 @@
       </c>
     </row>
     <row r="72" spans="1:7">
-      <c r="A72" s="13" t="n">
+      <c r="A72" s="7">
         <v>42390</v>
       </c>
       <c r="B72" t="s">
@@ -5459,7 +5415,7 @@
       </c>
     </row>
     <row r="73" spans="1:7">
-      <c r="A73" s="13" t="n">
+      <c r="A73" s="7">
         <v>42390</v>
       </c>
       <c r="B73" t="s">
@@ -5482,7 +5438,7 @@
       </c>
     </row>
     <row r="74" spans="1:7">
-      <c r="A74" s="13" t="n">
+      <c r="A74" s="7">
         <v>42390</v>
       </c>
       <c r="B74" t="s">
@@ -5505,7 +5461,7 @@
       </c>
     </row>
     <row r="75" spans="1:7">
-      <c r="A75" s="13" t="n">
+      <c r="A75" s="7">
         <v>42390</v>
       </c>
       <c r="B75" t="s">
@@ -5528,7 +5484,7 @@
       </c>
     </row>
     <row r="76" spans="1:7">
-      <c r="A76" s="13" t="n">
+      <c r="A76" s="7">
         <v>42390</v>
       </c>
       <c r="B76" t="s">
@@ -5551,7 +5507,7 @@
       </c>
     </row>
     <row r="77" spans="1:7">
-      <c r="A77" s="13" t="n">
+      <c r="A77" s="7">
         <v>42390</v>
       </c>
       <c r="B77" t="s">
@@ -5574,7 +5530,7 @@
       </c>
     </row>
     <row r="78" spans="1:7">
-      <c r="A78" s="13" t="n">
+      <c r="A78" s="7">
         <v>42390</v>
       </c>
       <c r="B78" t="s">
@@ -5597,7 +5553,7 @@
       </c>
     </row>
     <row r="79" spans="1:7">
-      <c r="A79" s="13" t="n">
+      <c r="A79" s="7">
         <v>42390</v>
       </c>
       <c r="B79" t="s">
@@ -5620,7 +5576,7 @@
       </c>
     </row>
     <row r="80" spans="1:7">
-      <c r="A80" s="13" t="n">
+      <c r="A80" s="7">
         <v>42390</v>
       </c>
       <c r="B80" t="s">
@@ -5643,7 +5599,7 @@
       </c>
     </row>
     <row r="81" spans="1:7">
-      <c r="A81" s="13" t="n">
+      <c r="A81" s="7">
         <v>42390</v>
       </c>
       <c r="B81" t="s">
@@ -5666,7 +5622,7 @@
       </c>
     </row>
     <row r="82" spans="1:7">
-      <c r="A82" s="13" t="n">
+      <c r="A82" s="7">
         <v>42390</v>
       </c>
       <c r="B82" t="s">
@@ -5689,7 +5645,7 @@
       </c>
     </row>
     <row r="83" spans="1:7">
-      <c r="A83" s="13" t="n">
+      <c r="A83" s="7">
         <v>42390</v>
       </c>
       <c r="B83" t="s">
@@ -5712,7 +5668,7 @@
       </c>
     </row>
     <row r="84" spans="1:7">
-      <c r="A84" s="13" t="n">
+      <c r="A84" s="7">
         <v>42390</v>
       </c>
       <c r="B84" t="s">
@@ -5735,7 +5691,7 @@
       </c>
     </row>
     <row r="85" spans="1:7">
-      <c r="A85" s="13" t="n">
+      <c r="A85" s="7">
         <v>42390</v>
       </c>
       <c r="B85" t="s">
@@ -5758,7 +5714,7 @@
       </c>
     </row>
     <row r="86" spans="1:7">
-      <c r="A86" s="13" t="n">
+      <c r="A86" s="7">
         <v>42390</v>
       </c>
       <c r="B86" t="s">
@@ -5781,7 +5737,7 @@
       </c>
     </row>
     <row r="87" spans="1:7">
-      <c r="A87" s="13" t="n">
+      <c r="A87" s="7">
         <v>42390</v>
       </c>
       <c r="B87" t="s">
@@ -5804,7 +5760,7 @@
       </c>
     </row>
     <row r="88" spans="1:7">
-      <c r="A88" s="13" t="n">
+      <c r="A88" s="7">
         <v>42390</v>
       </c>
       <c r="B88" t="s">
@@ -5827,7 +5783,7 @@
       </c>
     </row>
     <row r="89" spans="1:7">
-      <c r="A89" s="13" t="n">
+      <c r="A89" s="7">
         <v>42390</v>
       </c>
       <c r="B89" t="s">
@@ -5850,107 +5806,108 @@
       </c>
     </row>
     <row r="90" spans="1:7">
-      <c r="A90" s="9" t="n">
+      <c r="A90" s="3">
         <v>42390</v>
       </c>
-      <c r="B90" s="10" t="s">
+      <c r="B90" s="4" t="s">
         <v>485</v>
       </c>
-      <c r="C90" s="10" t="s"/>
-      <c r="D90" s="10" t="s">
+      <c r="C90" s="4"/>
+      <c r="D90" s="4" t="s">
         <v>486</v>
       </c>
-      <c r="E90" s="10" t="s">
+      <c r="E90" s="4" t="s">
         <v>487</v>
       </c>
-      <c r="F90" s="10" t="s">
+      <c r="F90" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="G90" s="10" t="s">
+      <c r="G90" s="4" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="91" spans="1:7">
-      <c r="A91" s="9" t="n">
+      <c r="A91" s="3">
         <v>42390</v>
       </c>
-      <c r="B91" s="10" t="s">
+      <c r="B91" s="4" t="s">
         <v>488</v>
       </c>
-      <c r="C91" s="10" t="s"/>
-      <c r="D91" s="10" t="s">
+      <c r="C91" s="4"/>
+      <c r="D91" s="4" t="s">
         <v>489</v>
       </c>
-      <c r="E91" s="10" t="s">
+      <c r="E91" s="4" t="s">
         <v>490</v>
       </c>
-      <c r="F91" s="10" t="s">
+      <c r="F91" s="4" t="s">
         <v>227</v>
       </c>
-      <c r="G91" s="10" t="s">
+      <c r="G91" s="4" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="92" spans="1:7">
-      <c r="A92" s="9" t="n">
+      <c r="A92" s="3">
         <v>42390</v>
       </c>
-      <c r="B92" s="10" t="s">
+      <c r="B92" s="4" t="s">
         <v>491</v>
       </c>
-      <c r="C92" s="10" t="s"/>
-      <c r="D92" s="10" t="s">
+      <c r="C92" s="4"/>
+      <c r="D92" s="4" t="s">
         <v>492</v>
       </c>
-      <c r="E92" s="10" t="s">
+      <c r="E92" s="4" t="s">
         <v>493</v>
       </c>
-      <c r="F92" s="10" t="s">
+      <c r="F92" s="4" t="s">
         <v>227</v>
       </c>
-      <c r="G92" s="10" t="s">
+      <c r="G92" s="4" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="93" spans="1:7">
-      <c r="A93" s="11" t="n">
+      <c r="A93" s="5">
         <v>42390</v>
       </c>
-      <c r="B93" s="12" t="s">
+      <c r="B93" s="6" t="s">
         <v>494</v>
       </c>
-      <c r="C93" s="12" t="s"/>
-      <c r="D93" s="12" t="s">
+      <c r="C93" s="6"/>
+      <c r="D93" s="6" t="s">
         <v>495</v>
       </c>
-      <c r="E93" s="12" t="s">
+      <c r="E93" s="6" t="s">
         <v>496</v>
       </c>
-      <c r="F93" s="12" t="s"/>
-      <c r="G93" s="12" t="s">
+      <c r="F93" s="6"/>
+      <c r="G93" s="6" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="94" spans="1:7">
-      <c r="A94" s="11" t="n">
+      <c r="A94" s="5">
         <v>42390</v>
       </c>
-      <c r="B94" s="12" t="s">
+      <c r="B94" s="6" t="s">
         <v>497</v>
       </c>
-      <c r="C94" s="12" t="s"/>
-      <c r="D94" s="12" t="s">
+      <c r="C94" s="6"/>
+      <c r="D94" s="6" t="s">
         <v>498</v>
       </c>
-      <c r="E94" s="12" t="s">
+      <c r="E94" s="6" t="s">
         <v>499</v>
       </c>
-      <c r="F94" s="12" t="s"/>
-      <c r="G94" s="12" t="s">
+      <c r="F94" s="6"/>
+      <c r="G94" s="6" t="s">
         <v>101</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add ActiveMQ to whiteList
</commit_message>
<xml_diff>
--- a/vulsList_20160128.xlsx
+++ b/vulsList_20160128.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="570" yWindow="465" windowWidth="8280" windowHeight="6960" activeTab="1"/>
+    <workbookView xWindow="570" yWindow="465" windowWidth="8280" windowHeight="6960"/>
   </bookViews>
   <sheets>
     <sheet name="whiteList" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="943" uniqueCount="500">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="944" uniqueCount="501">
   <si>
     <t>tech keywords</t>
   </si>
@@ -1517,6 +1517,10 @@
   </si>
   <si>
     <t>CVE-2015-8705</t>
+  </si>
+  <si>
+    <t>activemq</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1899,10 +1903,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A25"/>
+  <dimension ref="A1:A26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
@@ -2038,6 +2042,11 @@
         <v>32</v>
       </c>
     </row>
+    <row r="26" spans="1:1">
+      <c r="A26" s="1" t="s">
+        <v>500</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2049,7 +2058,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>

</xml_diff>